<commit_message>
this is modified xls file
</commit_message>
<xml_diff>
--- a/testcase.xlsx
+++ b/testcase.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LIKHAN\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LIKHAN\Desktop\Lab final\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -144,7 +144,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve"> website</t>
+      <t xml:space="preserve"> website.</t>
     </r>
   </si>
 </sst>
@@ -250,9 +250,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -263,6 +260,9 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -547,7 +547,7 @@
   <dimension ref="A1:K16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J14" sqref="I14:J14"/>
+      <selection activeCell="A2" sqref="A2:A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -589,7 +589,7 @@
       </c>
     </row>
     <row r="2" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="6" t="s">
+      <c r="A2" s="10" t="s">
         <v>32</v>
       </c>
       <c r="B2" t="s">
@@ -615,7 +615,7 @@
       </c>
     </row>
     <row r="3" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="6"/>
+      <c r="A3" s="10"/>
       <c r="B3" t="s">
         <v>14</v>
       </c>
@@ -631,10 +631,10 @@
       <c r="F3" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="G3" s="7" t="s">
+      <c r="G3" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="H3" s="8" t="s">
+      <c r="H3" s="7" t="s">
         <v>19</v>
       </c>
       <c r="I3" s="3"/>
@@ -642,7 +642,7 @@
       <c r="K3" s="3"/>
     </row>
     <row r="4" spans="1:11" ht="45" x14ac:dyDescent="0.25">
-      <c r="A4" s="6"/>
+      <c r="A4" s="10"/>
       <c r="B4" t="s">
         <v>20</v>
       </c>
@@ -658,10 +658,10 @@
       <c r="F4" t="s">
         <v>23</v>
       </c>
-      <c r="G4" s="7" t="s">
+      <c r="G4" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="H4" s="9" t="s">
+      <c r="H4" s="8" t="s">
         <v>19</v>
       </c>
       <c r="I4" s="3"/>
@@ -669,7 +669,7 @@
       <c r="K4" s="3"/>
     </row>
     <row r="5" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="6"/>
+      <c r="A5" s="10"/>
       <c r="B5" t="s">
         <v>25</v>
       </c>
@@ -690,7 +690,7 @@
       </c>
     </row>
     <row r="6" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="6"/>
+      <c r="A6" s="10"/>
       <c r="B6" s="3" t="s">
         <v>28</v>
       </c>
@@ -706,12 +706,12 @@
       <c r="F6" t="s">
         <v>23</v>
       </c>
-      <c r="H6" s="10" t="s">
+      <c r="H6" s="9" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A7" s="6"/>
+      <c r="A7" s="10"/>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B14" s="3"/>

</xml_diff>